<commit_message>
fixed bugs and first results obtained
</commit_message>
<xml_diff>
--- a/Preguntas.xlsx
+++ b/Preguntas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\Master\Asignaturas\Lingüistica\Practica 3\QA-System-Pokemon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\UPM\Actual\IngLinguistica\P3\QA-System-Pokemon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69799D8B-B981-42CB-81BF-4AA7B195612B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D64DA0-DC29-49CE-AFF6-7156C2120113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20595" yWindow="1275" windowWidth="44970" windowHeight="21000" xr2:uid="{15D36274-4D20-4D64-BA55-4854925D7C09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15D36274-4D20-4D64-BA55-4854925D7C09}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -56,33 +56,12 @@
     <t>Habilidades</t>
   </si>
   <si>
-    <t>Generación</t>
-  </si>
-  <si>
     <t>Movimientos</t>
   </si>
   <si>
-    <t>¿Qué número de la pokedex es #pokemon#?, ¿Qué entrada es #pokemon# en la pokedex?, ¿Como se identifica a #pokemon#?, ¿Cuál es el identificador a #pokemon#?, ¿En qué página esta #pokemon#?</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Obtención</t>
-  </si>
-  <si>
-    <t>¿Cuál es la descripción de #pokemon#?, ¿Como es #pokemon#?, ¿Como describirías a #pokemon#?</t>
-  </si>
-  <si>
     <t>¿De qué tipo es #pokemon#?, ¿Con que hace más daño #pokemon#?, ¿Qué movimientos potencia #pokemon#?, ¿Con que pega más #pokemon#?</t>
   </si>
   <si>
-    <t>¿Cuánto pesa #pokemon#?, ¿Como de pesado es #pokemon#?</t>
-  </si>
-  <si>
-    <t>¿Cuánto mide #pokemon#?, ¿Como de alto es #pokemon#?, ¿Como de grande es #pokemon#?</t>
-  </si>
-  <si>
     <t>¿Es #pokemon# legendario?, ¿Es #pokemon# especial?, ¿Es #pokemon# único?, ¿#pokemon# proviene de la mitología?</t>
   </si>
   <si>
@@ -98,27 +77,15 @@
     <t>¿Cuál es la cadena evolutiva de #pokemon#?, ¿Cuál es la evolución #pokemon#?, ¿Cuáles son las evoluciones de #pokemon#?, ¿Cuáles son las preevoluciones de #pokemon#?, ¿#pokemon# evoluciona?</t>
   </si>
   <si>
-    <t>¿Como se obtiene a #pokemon#?, ¿Como/Donde se consigue a #pokemon#?, ¿Como/Donde se captura a #pokemon#?</t>
-  </si>
-  <si>
-    <t>¿Qué movimientos aprende #pokemon#?, ¿Que aprende #pokemon#?, ¿Qué ataques puede hacer #pokemon#?, ¿Con que puede atacar #pokemon#?</t>
-  </si>
-  <si>
     <t>¿Cuál es el hábitat de #pokemon#?, ¿Dónde vive #pokemon#?, ¿Dónde nace #pokemon#?, ¿En qué lugar vive #pokemon#?</t>
   </si>
   <si>
-    <t>¿Cuál es el ratio de captura de #pokemon#?, ¿Es fácil capturar a #pokemon#?, ¿Es complicado capturar a #pokemon#?, ¿Como de probable es capturar a #pokemon#?</t>
-  </si>
-  <si>
     <t>Campo</t>
   </si>
   <si>
     <t>Preguntas</t>
   </si>
   <si>
-    <t>¿A que es débil #pokemon#?, ¿Qué le hace mucho daño a #pokemon#?, ¿Qué tiene que evitar #pokemon#?, ¿Que debilita o hiere a #pokemon#?, ¿Qué le afecta a #pokemon#?, ¿Cómo debilitar a pikachu?</t>
-  </si>
-  <si>
     <t>N_Pokedex</t>
   </si>
   <si>
@@ -132,13 +99,46 @@
   </si>
   <si>
     <t>Ratio_de_Captura</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Obtencion</t>
+  </si>
+  <si>
+    <t>Generacion</t>
+  </si>
+  <si>
+    <t>¿Qué número de la pokedex es #pokemon#?, ¿Qué entrada es #pokemon# en la pokedex?, ¿Cómo se identifica a #pokemon#?, ¿Cuál es el identificador a #pokemon#?, ¿En qué página esta #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿Cuál es la descripción de #pokemon#?, ¿Cómo es #pokemon#?, ¿Cómo describirías a #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿A que es débil #pokemon#?, ¿Qué le hace mucho daño a #pokemon#?, ¿Qué tiene que evitar #pokemon#?, ¿Qué debilita o hiere a #pokemon#?, ¿Qué le afecta a #pokemon#?, ¿Cómo debilitar a pikachu?</t>
+  </si>
+  <si>
+    <t>¿Cuánto pesa #pokemon#?, ¿Cómo de pesado es #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿Cuánto mide #pokemon#?, ¿Cómo de alto es #pokemon#?, ¿Cómo de grande es #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿Cómo se obtiene a #pokemon#?, ¿Cómo se consigue a #pokemon#?, ¿Dónde se consigue a #pokemon#?, ¿Cómo se captura a #pokemon#?, ¿Dónde se captura a #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el ratio de captura de #pokemon#?, ¿Es fácil capturar a #pokemon#?, ¿Es complicado capturar a #pokemon#?, ¿Cómo de probable es capturar a #pokemon#?</t>
+  </si>
+  <si>
+    <t>¿Qué movimientos aprende #pokemon#?, ¿Qué aprende #pokemon#?, ¿Qué ataques puede hacer #pokemon#?, ¿Con que puede atacar #pokemon#?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,15 +148,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,12 +190,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +511,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,26 +522,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -560,7 +549,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -576,7 +565,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +581,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,63 +589,63 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
+      <c r="A10" t="s">
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
+      <c r="A13" t="s">
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>